<commit_message>
changed batch inference logic
</commit_message>
<xml_diff>
--- a/result/baseline_aadhar_back.xlsx
+++ b/result/baseline_aadhar_back.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\M.Tech Sem 3\NLP\Project\NetraAadhar\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F989A291-E2A4-4F61-8EA8-34C78453CF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E28A8383-63C1-4847-AB6A-BEE99335AE55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="21520" windowHeight="12800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="657">
   <si>
     <t>file_name</t>
   </si>
@@ -1992,6 +1992,9 @@
   </si>
   <si>
     <t>Wrong</t>
+  </si>
+  <si>
+    <t>aadhar_front</t>
   </si>
 </sst>
 </file>
@@ -4891,7 +4894,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -4903,6 +4906,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>656</v>
+      </c>
       <c r="B1" t="s">
         <v>649</v>
       </c>

</xml_diff>